<commit_message>
latest trialsheets for pilot2
</commit_message>
<xml_diff>
--- a/megStimMovie1.xlsx
+++ b/megStimMovie1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +471,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -495,16 +495,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -519,16 +519,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -543,16 +543,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -567,16 +567,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -591,16 +591,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -615,16 +615,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -639,16 +639,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -663,16 +663,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -687,16 +687,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -711,16 +711,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -735,16 +735,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -759,16 +759,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -783,16 +783,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -807,16 +807,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -831,16 +831,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -855,16 +855,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -879,16 +879,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -903,16 +903,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -927,16 +927,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -951,19 +951,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -975,19 +975,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -999,16 +999,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1023,16 +1023,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1047,16 +1047,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1071,16 +1071,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1095,16 +1095,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1119,19 +1119,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1143,19 +1143,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1167,16 +1167,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1191,16 +1191,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1215,16 +1215,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1239,16 +1239,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1263,16 +1263,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1287,16 +1287,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1311,19 +1311,19 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1331,20 +1331,20 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1359,16 +1359,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1383,16 +1383,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1407,16 +1407,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -1431,16 +1431,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -1455,19 +1455,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1479,19 +1479,19 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1503,16 +1503,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -1527,22 +1527,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1551,22 +1551,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1575,16 +1575,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -1599,19 +1599,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1623,16 +1623,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -1647,19 +1647,19 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1671,16 +1671,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -1695,16 +1695,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -1719,16 +1719,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -1743,16 +1743,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -1767,19 +1767,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -1791,16 +1791,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -1815,16 +1815,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -1839,16 +1839,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -1863,16 +1863,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -1887,16 +1887,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -1911,16 +1911,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -1935,16 +1935,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -1959,19 +1959,19 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -1983,16 +1983,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -2007,19 +2007,19 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2031,16 +2031,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -2055,16 +2055,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -2079,16 +2079,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -2103,16 +2103,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -2127,19 +2127,19 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -2151,16 +2151,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -2175,19 +2175,19 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -2199,16 +2199,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -2223,16 +2223,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
@@ -2247,16 +2247,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -2271,16 +2271,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -2295,19 +2295,19 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2319,16 +2319,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -2343,22 +2343,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2367,22 +2367,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -2391,16 +2391,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -2415,16 +2415,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -2439,16 +2439,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -2463,19 +2463,19 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2487,16 +2487,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -2511,16 +2511,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
@@ -2535,19 +2535,19 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -2559,16 +2559,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -2583,16 +2583,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -2607,46 +2607,46 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
+        <v>5</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
         <v>6</v>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>0247_Right</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>12</v>
-      </c>
       <c r="E92" t="n">
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -2655,16 +2655,16 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -2679,16 +2679,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -2703,16 +2703,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -2727,19 +2727,19 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -2751,16 +2751,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -2775,16 +2775,16 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -2799,19 +2799,19 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -2823,16 +2823,16 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -2847,16 +2847,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0247_Right</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
@@ -2871,22 +2871,22 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -2895,22 +2895,22 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -2919,19 +2919,19 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -2943,16 +2943,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -2967,16 +2967,16 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E106" t="n">
         <v>0</v>
@@ -2991,19 +2991,19 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -3015,16 +3015,16 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -3039,16 +3039,16 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -3059,20 +3059,20 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>0337_Right</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -3087,16 +3087,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>0247_Right</t>
+          <t>0337_Right</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -3111,19 +3111,19 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>0157_Right</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
@@ -3135,16 +3135,16 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>0022_Left</t>
+          <t>0122_Left</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
@@ -3159,16 +3159,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>0337_Left</t>
+          <t>0292_Left</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -3183,16 +3183,16 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>0122_Left</t>
+          <t>0122_Right</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E115" t="n">
         <v>0</v>
@@ -3207,16 +3207,16 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>0202_Left</t>
+          <t>0337_Left</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
@@ -3231,16 +3231,16 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>0157_Left</t>
+          <t>0202_Right</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
@@ -3255,16 +3255,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>0067_Right</t>
+          <t>0067_Left</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E118" t="n">
         <v>0</v>
@@ -3279,16 +3279,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>0292_Left</t>
+          <t>0022_Right</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E119" t="n">
         <v>0</v>
@@ -3303,19 +3303,19 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0292_Right</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F120" t="n">
         <v>0</v>
@@ -3327,16 +3327,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>0067_Left</t>
+          <t>0067_Right</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
@@ -3351,19 +3351,19 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>0247_Left</t>
+          <t>0157_Left</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
@@ -3375,16 +3375,16 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>0202_Right</t>
+          <t>0022_Left</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E123" t="n">
         <v>0</v>
@@ -3399,16 +3399,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>0292_Right</t>
+          <t>0247_Left</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E124" t="n">
         <v>0</v>
@@ -3423,22 +3423,22 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>0022_Right</t>
+          <t>0157_Right</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -3447,16 +3447,16 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>0122_Right</t>
+          <t>0202_Left</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E126" t="n">
         <v>0</v>
@@ -3471,21 +3471,1749 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0247_Right</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>12</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>8</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0202_Right</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>10</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>8</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0067_Left</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>17</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>8</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0337_Left</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>15</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>8</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>6</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>8</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
           <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr">
+      <c r="C132" t="inlineStr">
         <is>
           <t>0157_Right</t>
         </is>
       </c>
-      <c r="D127" t="n">
+      <c r="D132" t="n">
         <v>8</v>
       </c>
-      <c r="E127" t="n">
-        <v>0</v>
-      </c>
-      <c r="F127" t="n">
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>8</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>0337_Right</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>16</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>8</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0122_Left</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>5</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>8</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0022_Left</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>8</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0022_Right</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>2</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>8</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0067_Right</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>4</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>8</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0292_Left</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>13</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>8</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0067_Left</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>3</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>8</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0202_Left</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>9</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>8</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0292_Right</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>14</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>8</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0157_Left</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>7</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>8</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>11</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>8</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>17</v>
+      </c>
+      <c r="E144" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>8</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0247_Right</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>12</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>9</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0157_Left</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>7</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>9</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0292_Left</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>13</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0</v>
+      </c>
+      <c r="F147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>9</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0247_Right</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>12</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>9</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>11</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>9</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0067_Right</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>4</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>9</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>0337_Left</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>15</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>9</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>17</v>
+      </c>
+      <c r="E152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>9</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0022_Left</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>1</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0</v>
+      </c>
+      <c r="F153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>9</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0292_Right</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>14</v>
+      </c>
+      <c r="E154" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>9</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>0202_Left</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>9</v>
+      </c>
+      <c r="E155" t="n">
+        <v>0</v>
+      </c>
+      <c r="F155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>9</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>6</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>9</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>0202_Right</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>10</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>9</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0337_Right</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>16</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>9</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0067_Left</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>3</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0</v>
+      </c>
+      <c r="F159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>9</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>17</v>
+      </c>
+      <c r="E160" t="n">
+        <v>1</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>9</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0157_Right</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>8</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>9</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0022_Right</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>2</v>
+      </c>
+      <c r="E162" t="n">
+        <v>0</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>9</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0122_Left</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>5</v>
+      </c>
+      <c r="E163" t="n">
+        <v>0</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>10</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0202_Right</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>10</v>
+      </c>
+      <c r="E164" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>10</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>0157_Left</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>7</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>10</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0292_Right</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>14</v>
+      </c>
+      <c r="E166" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>10</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0067_Right</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>4</v>
+      </c>
+      <c r="E167" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>10</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>0157_Left</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>17</v>
+      </c>
+      <c r="E168" t="n">
+        <v>1</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>10</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0067_Left</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>3</v>
+      </c>
+      <c r="E169" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>10</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0157_Right</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>8</v>
+      </c>
+      <c r="E170" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>10</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>0337_Right</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>16</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>10</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>6</v>
+      </c>
+      <c r="E172" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>10</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>0292_Left</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>13</v>
+      </c>
+      <c r="E173" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>10</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>0202_Left</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>9</v>
+      </c>
+      <c r="E174" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>10</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>11</v>
+      </c>
+      <c r="E175" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>10</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>17</v>
+      </c>
+      <c r="E176" t="n">
+        <v>1</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>10</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>0122_Left</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>5</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>10</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>0247_Right</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>12</v>
+      </c>
+      <c r="E178" t="n">
+        <v>0</v>
+      </c>
+      <c r="F178" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>10</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>0022_Right</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>2</v>
+      </c>
+      <c r="E179" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>10</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>0022_Left</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>10</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>0337_Left</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>15</v>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>11</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Right.png</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>0157_Right</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>8</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>11</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>6</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>11</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Right.png</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>0122_Right</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>17</v>
+      </c>
+      <c r="E184" t="n">
+        <v>1</v>
+      </c>
+      <c r="F184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>11</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Left.png</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>0202_Left</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>9</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>11</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Right.png</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>0337_Right</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>16</v>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>11</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Left.png</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>0292_Left</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>13</v>
+      </c>
+      <c r="E187" t="n">
+        <v>0</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>11</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0292_Right.png</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>0292_Right</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>14</v>
+      </c>
+      <c r="E188" t="n">
+        <v>0</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>11</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Right.png</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>0067_Right</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>4</v>
+      </c>
+      <c r="E189" t="n">
+        <v>0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>11</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Left.png</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>0247_Left</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>11</v>
+      </c>
+      <c r="E190" t="n">
+        <v>0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>11</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>0247_Right</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>12</v>
+      </c>
+      <c r="E191" t="n">
+        <v>0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>11</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0247_Right.png</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>0337_Left</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>17</v>
+      </c>
+      <c r="E192" t="n">
+        <v>1</v>
+      </c>
+      <c r="F192" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>11</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0337_Left.png</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>0337_Left</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>15</v>
+      </c>
+      <c r="E193" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>11</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0202_Right.png</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>0202_Right</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>10</v>
+      </c>
+      <c r="E194" t="n">
+        <v>0</v>
+      </c>
+      <c r="F194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>11</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Left.png</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>0022_Left</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>1</v>
+      </c>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>11</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0022_Right.png</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>0022_Right</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>2</v>
+      </c>
+      <c r="E196" t="n">
+        <v>0</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>11</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0067_Left.png</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>0067_Left</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>3</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0</v>
+      </c>
+      <c r="F197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>11</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0122_Left.png</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>0122_Left</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>5</v>
+      </c>
+      <c r="E198" t="n">
+        <v>0</v>
+      </c>
+      <c r="F198" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>11</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>C:/Users/meglab/EExperiments/Sebastian/BlenderPilot/Stimuli/0157_Left.png</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>0157_Left</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>7</v>
+      </c>
+      <c r="E199" t="n">
+        <v>0</v>
+      </c>
+      <c r="F199" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>